<commit_message>
aggiornamento fogli di calcolo
</commit_message>
<xml_diff>
--- a/FogliCalcolo/ElevatoreTazze/ElevatoreTazze.xlsx
+++ b/FogliCalcolo/ElevatoreTazze/ElevatoreTazze.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Uni\Impianti meccanici\MaterialeEsame\FogliCalcolo\ElevatoreTazze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210B91C4-BA8B-4867-A86A-53517AC168EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66F2C6F-4C42-416E-A369-EDA273A0DF73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B46271C-1738-49D0-9144-B24F73B3C7E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Foglio1!$A$1:$Q$52</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -728,7 +731,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -755,6 +758,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -764,27 +779,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2606,10 +2610,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39681D44-E619-4003-BE77-2BCEF7DD284F}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2704,11 +2711,11 @@
       <c r="D8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="29"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="26"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C9" s="6"/>
@@ -2742,16 +2749,16 @@
       <c r="C12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="20">
         <v>9</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="20">
         <v>7.2</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="20">
         <v>4</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="20">
         <v>4</v>
       </c>
       <c r="H12" s="7" t="s">
@@ -2765,19 +2772,19 @@
       <c r="C13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="20">
         <f>105*0.001</f>
         <v>0.105</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="20">
         <f t="shared" ref="E13:G13" si="0">105*0.001</f>
         <v>0.105</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="20">
         <f t="shared" si="0"/>
         <v>0.105</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="20">
         <f t="shared" si="0"/>
         <v>0.105</v>
       </c>
@@ -2795,19 +2802,19 @@
       <c r="C14" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="20">
         <f>308*0.001</f>
         <v>0.308</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="20">
         <f t="shared" ref="E14:G14" si="1">308*0.001</f>
         <v>0.308</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="20">
         <f t="shared" si="1"/>
         <v>0.308</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="20">
         <f t="shared" si="1"/>
         <v>0.308</v>
       </c>
@@ -2843,19 +2850,19 @@
       <c r="C16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="21">
         <f>D13*D15</f>
         <v>0.63</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="21">
         <f t="shared" ref="E16:G16" si="2">E13*E15</f>
         <v>0.84</v>
       </c>
-      <c r="F16" s="24">
+      <c r="F16" s="21">
         <f t="shared" si="2"/>
         <v>1.05</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16" s="21">
         <f t="shared" si="2"/>
         <v>0.52500000000000002</v>
       </c>
@@ -2936,7 +2943,7 @@
         <v>25</v>
       </c>
       <c r="H20" s="7"/>
-      <c r="I20" s="29" t="s">
+      <c r="I20" s="26" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2969,32 +2976,32 @@
       <c r="B22" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="33">
+      <c r="D22" s="28">
         <f>(9.81*(D21/D18)^2-D21)/D21</f>
         <v>1.2946010876880731</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E22" s="28">
         <f>(9.81*(E21/E18)^2-E21)/E21</f>
         <v>3.2570489459633242E-2</v>
       </c>
-      <c r="F22" s="33">
+      <c r="F22" s="28">
         <f>(9.81*(F21/F18)^2-F21)/F21</f>
         <v>-0.7552425506466055</v>
       </c>
-      <c r="G22" s="33">
+      <c r="G22" s="28">
         <f>(9.81*(G21/G18)^2-G21)/G21</f>
         <v>0.3597636075188585</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="1"/>
-      <c r="M22" s="29"/>
+      <c r="M22" s="26"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
-      <c r="C23" s="31"/>
+      <c r="C23" s="34"/>
       <c r="D23" s="14">
         <f>9.81*(D21/D18)^2</f>
         <v>0.46014835296729151</v>
@@ -3015,20 +3022,20 @@
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="35" t="str">
+      <c r="C24" s="35"/>
+      <c r="D24" s="29" t="str">
         <f>IF(D22&lt;0,"centrifugo","gravitazionale")</f>
         <v>gravitazionale</v>
       </c>
-      <c r="E24" s="35" t="str">
+      <c r="E24" s="29" t="str">
         <f t="shared" ref="E24:G24" si="3">IF(E22&lt;0,"centrifugo","gravitazionale")</f>
         <v>gravitazionale</v>
       </c>
-      <c r="F24" s="35" t="str">
+      <c r="F24" s="29" t="str">
         <f t="shared" si="3"/>
         <v>centrifugo</v>
       </c>
-      <c r="G24" s="35" t="str">
+      <c r="G24" s="29" t="str">
         <f t="shared" si="3"/>
         <v>gravitazionale</v>
       </c>
@@ -3174,15 +3181,15 @@
     </row>
     <row r="31" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="22"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="32"/>
     </row>
     <row r="33" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B33" s="5" t="s">
@@ -3191,16 +3198,16 @@
       <c r="C33" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="25">
+      <c r="D33" s="22">
         <v>2.5</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="22">
         <v>2.5</v>
       </c>
-      <c r="F33" s="25">
+      <c r="F33" s="22">
         <v>2.5</v>
       </c>
-      <c r="G33" s="25">
+      <c r="G33" s="22">
         <v>2.5</v>
       </c>
       <c r="H33" s="7" t="s">
@@ -3214,16 +3221,16 @@
       <c r="C34" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D34" s="25">
+      <c r="D34" s="22">
         <v>9</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="22">
         <v>9</v>
       </c>
-      <c r="F34" s="25">
+      <c r="F34" s="22">
         <v>8</v>
       </c>
-      <c r="G34" s="25">
+      <c r="G34" s="22">
         <v>8</v>
       </c>
       <c r="H34" s="7" t="s">
@@ -3237,16 +3244,16 @@
       <c r="C35" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D35" s="25">
+      <c r="D35" s="22">
         <v>50</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="22">
         <v>50</v>
       </c>
-      <c r="F35" s="25">
+      <c r="F35" s="22">
         <v>50</v>
       </c>
-      <c r="G35" s="25">
+      <c r="G35" s="22">
         <v>50</v>
       </c>
       <c r="H35" s="7" t="s">
@@ -3257,7 +3264,7 @@
       <c r="B36" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="21" t="s">
         <v>64</v>
       </c>
       <c r="D36" s="6">
@@ -3284,7 +3291,7 @@
       <c r="B37" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="21" t="s">
         <v>65</v>
       </c>
       <c r="D37" s="6">
@@ -3311,7 +3318,7 @@
       <c r="B38" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="21" t="s">
         <v>66</v>
       </c>
       <c r="D38" s="6">
@@ -3338,7 +3345,7 @@
       <c r="B39" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="21" t="s">
         <v>67</v>
       </c>
       <c r="D39" s="6">
@@ -3365,7 +3372,7 @@
       <c r="B40" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C40" s="21" t="s">
         <v>68</v>
       </c>
       <c r="D40" s="6">
@@ -3392,7 +3399,7 @@
       <c r="B41" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="21" t="s">
         <v>69</v>
       </c>
       <c r="D41" s="6">
@@ -3415,7 +3422,7 @@
       <c r="B42" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="21" t="s">
         <v>70</v>
       </c>
       <c r="D42" s="6">
@@ -3434,7 +3441,7 @@
         <f>1.4*$C$4*9.81</f>
         <v>824.04000000000008</v>
       </c>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="27" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3442,7 +3449,7 @@
       <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="24" t="s">
+      <c r="C43" s="21" t="s">
         <v>71</v>
       </c>
       <c r="D43" s="14">
@@ -3469,7 +3476,7 @@
       <c r="B44" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C44" s="24" t="s">
+      <c r="C44" s="21" t="s">
         <v>72</v>
       </c>
       <c r="D44" s="14">
@@ -3502,39 +3509,39 @@
       <c r="H45" s="7"/>
     </row>
     <row r="46" spans="2:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B46" s="28"/>
+      <c r="B46" s="25"/>
       <c r="C46" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D46" s="23">
+      <c r="D46" s="20">
         <v>0.9</v>
       </c>
-      <c r="E46" s="23">
+      <c r="E46" s="20">
         <v>0.9</v>
       </c>
-      <c r="F46" s="23">
+      <c r="F46" s="20">
         <v>0.9</v>
       </c>
-      <c r="G46" s="23">
+      <c r="G46" s="20">
         <v>0.9</v>
       </c>
       <c r="H46" s="7"/>
     </row>
     <row r="47" spans="2:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B47" s="28"/>
+      <c r="B47" s="25"/>
       <c r="C47" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D47" s="23">
+      <c r="D47" s="20">
         <v>0.8</v>
       </c>
-      <c r="E47" s="23">
+      <c r="E47" s="20">
         <v>0.8</v>
       </c>
-      <c r="F47" s="23">
+      <c r="F47" s="20">
         <v>0.8</v>
       </c>
-      <c r="G47" s="23">
+      <c r="G47" s="20">
         <v>0.8</v>
       </c>
       <c r="H47" s="7"/>
@@ -3552,7 +3559,7 @@
         <f>E44*E18/(E46*E47)</f>
         <v>6.3456147548010966</v>
       </c>
-      <c r="F48" s="15">
+      <c r="F48" s="36">
         <f>F44*F18/(F46*F47)</f>
         <v>9.8967708333333295</v>
       </c>
@@ -3570,7 +3577,7 @@
     <mergeCell ref="C22:C24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sistemato elevatore a tazze
</commit_message>
<xml_diff>
--- a/FogliCalcolo/ElevatoreTazze/ElevatoreTazze.xlsx
+++ b/FogliCalcolo/ElevatoreTazze/ElevatoreTazze.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Uni\Impianti meccanici\MaterialeEsame\FogliCalcolo\ElevatoreTazze\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giona\Desktop\git\ImpiantiMeccanici\FogliCalcolo\ElevatoreTazze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66F2C6F-4C42-416E-A369-EDA273A0DF73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788374F0-C076-4726-9DDD-AD2084825CDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B46271C-1738-49D0-9144-B24F73B3C7E6}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="78">
   <si>
     <t>pc</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>Dimensioni</t>
-  </si>
-  <si>
-    <t>N° anelli</t>
   </si>
   <si>
     <t xml:space="preserve">N° tazze </t>
@@ -169,9 +166,6 @@
     <t>massa tazza</t>
   </si>
   <si>
-    <t>peso catene</t>
-  </si>
-  <si>
     <t>peso tazze</t>
   </si>
   <si>
@@ -187,9 +181,6 @@
     <t>peso materiale</t>
   </si>
   <si>
-    <t>peso pulegge inf.</t>
-  </si>
-  <si>
     <t>massa puleggia</t>
   </si>
   <si>
@@ -215,9 +206,6 @@
   </si>
   <si>
     <t>Dati</t>
-  </si>
-  <si>
-    <t>N° denti ruota da catalogo (pag 22)</t>
   </si>
   <si>
     <r>
@@ -528,6 +516,21 @@
   </si>
   <si>
     <t xml:space="preserve">scarto </t>
+  </si>
+  <si>
+    <t>N° denti ruota da catalogo (verificare compatibilità puleggia - catena)</t>
+  </si>
+  <si>
+    <t>OM nel grafico pag. 412 Monte</t>
+  </si>
+  <si>
+    <t>N° anelli totale</t>
+  </si>
+  <si>
+    <t>peso puleggia inf.</t>
+  </si>
+  <si>
+    <t>peso catena</t>
   </si>
 </sst>
 </file>
@@ -731,7 +734,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -770,6 +773,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -788,7 +792,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -878,7 +887,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -980,16 +989,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2383.83</c:v>
+                  <c:v>1191.915</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1462.0824</c:v>
+                  <c:v>731.0412</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>635.68799999999999</c:v>
+                  <c:v>317.84399999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1342.0080000000003</c:v>
+                  <c:v>671.00400000000013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1052,16 +1061,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>741.67650000000003</c:v>
+                  <c:v>227.59200000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>674.48761999999999</c:v>
+                  <c:v>199.27543500000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>592.46640000000002</c:v>
+                  <c:v>168.43770000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>730.76240000000007</c:v>
+                  <c:v>211.84695000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1175,7 +1184,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>peso catene</c:v>
+                        <c:v>peso catena</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1206,16 +1215,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>8820</c:v>
+                        <c:v>2207.25</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>9016</c:v>
+                        <c:v>2256.3000000000002</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>8820</c:v>
+                        <c:v>2207.25</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>9310</c:v>
+                        <c:v>2329.875</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1298,16 +1307,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>2648.7000000000003</c:v>
+                        <c:v>662.17500000000007</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>2030.67</c:v>
+                        <c:v>507.66750000000002</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>1412.64</c:v>
+                        <c:v>353.16</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>2982.2400000000002</c:v>
+                        <c:v>745.56000000000006</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1335,7 +1344,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>peso pulegge inf.</c:v>
+                        <c:v>peso puleggia inf.</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1390,16 +1399,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>981</c:v>
+                        <c:v>490.5</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>981</c:v>
+                        <c:v>490.5</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>981</c:v>
+                        <c:v>490.5</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>981</c:v>
+                        <c:v>490.5</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1482,16 +1491,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>0</c:v>
+                        <c:v>2000</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0</c:v>
+                        <c:v>2001</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0</c:v>
+                        <c:v>2002</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0</c:v>
+                        <c:v>2003</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1541,7 +1550,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="704943728"/>
@@ -1623,7 +1632,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="it-IT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1655,7 +1664,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="704944976"/>
@@ -1697,7 +1706,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1727,7 +1736,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="it-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2615,8 +2624,8 @@
   </sheetPr>
   <dimension ref="B1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2634,7 +2643,7 @@
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="13"/>
@@ -2649,7 +2658,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -2662,7 +2671,7 @@
         <v>60</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -2675,7 +2684,7 @@
         <v>1800</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -2695,7 +2704,7 @@
         <v>0.5</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -2709,7 +2718,7 @@
         <v>8.5</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="23"/>
       <c r="F8" s="24"/>
@@ -2762,7 +2771,7 @@
         <v>4</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -2789,10 +2798,10 @@
         <v>0.105</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -2800,7 +2809,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D14" s="20">
         <f>308*0.001</f>
@@ -2819,15 +2828,15 @@
         <v>0.308</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="D15" s="16">
         <v>6</v>
@@ -2867,7 +2876,7 @@
         <v>0.52500000000000002</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
@@ -2913,7 +2922,7 @@
         <v>1.7361111111111109</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
@@ -2943,9 +2952,12 @@
         <v>25</v>
       </c>
       <c r="H20" s="7"/>
-      <c r="I20" s="26" t="s">
-        <v>55</v>
-      </c>
+      <c r="I20" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
@@ -2969,14 +2981,14 @@
         <v>0.41778172561622523</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="34" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="28">
@@ -3001,7 +3013,7 @@
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
-      <c r="C23" s="34"/>
+      <c r="C23" s="35"/>
       <c r="D23" s="14">
         <f>9.81*(D21/D18)^2</f>
         <v>0.46014835296729151</v>
@@ -3019,10 +3031,13 @@
         <v>0.56808438637937231</v>
       </c>
       <c r="H23" s="7"/>
+      <c r="I23" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="C24" s="35"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="29" t="str">
         <f>IF(D22&lt;0,"centrifugo","gravitazionale")</f>
         <v>gravitazionale</v>
@@ -3054,7 +3069,7 @@
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="16">
@@ -3071,15 +3086,15 @@
       </c>
       <c r="H26" s="7"/>
       <c r="I26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="2:13" ht="18" x14ac:dyDescent="0.35">
       <c r="B27" s="5" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D27" s="6">
         <f>_xlfn.CEILING.MATH((2*$C$8)/D13)+D20+D26</f>
@@ -3101,10 +3116,10 @@
     </row>
     <row r="28" spans="2:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D28" s="19">
         <f>D27/D15</f>
@@ -3124,15 +3139,15 @@
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="2:13" ht="18" x14ac:dyDescent="0.35">
       <c r="B29" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D29" s="14">
         <f>D27*D13</f>
@@ -3151,12 +3166,12 @@
         <v>19.95</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="15">
@@ -3176,27 +3191,27 @@
         <v>8.6624999999999996</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="32"/>
+      <c r="B32" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="33"/>
     </row>
     <row r="33" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B33" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D33" s="22">
         <v>2.5</v>
@@ -3211,15 +3226,15 @@
         <v>2.5</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B34" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D34" s="22">
         <v>9</v>
@@ -3234,15 +3249,15 @@
         <v>8</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B35" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D35" s="22">
         <v>50</v>
@@ -3257,246 +3272,246 @@
         <v>50</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B36" s="5" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D36" s="6">
-        <f>D33*D27*2*9.8</f>
-        <v>8820</v>
+        <f>D33*D27/2*9.81</f>
+        <v>2207.25</v>
       </c>
       <c r="E36" s="6">
-        <f>E33*E27*2*9.8</f>
-        <v>9016</v>
+        <f t="shared" ref="E36:G36" si="4">E33*E27/2*9.81</f>
+        <v>2256.3000000000002</v>
       </c>
       <c r="F36" s="6">
-        <f>F33*F27*2*9.8</f>
-        <v>8820</v>
+        <f t="shared" si="4"/>
+        <v>2207.25</v>
       </c>
       <c r="G36" s="6">
-        <f>G33*G27*2*9.8</f>
-        <v>9310</v>
+        <f t="shared" si="4"/>
+        <v>2329.875</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B37" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D37" s="6">
-        <f>D34*D28*9.81</f>
-        <v>2648.7000000000003</v>
+        <f>D34/2*D28/2*9.81</f>
+        <v>662.17500000000007</v>
       </c>
       <c r="E37" s="6">
-        <f>E34*E28*9.81</f>
-        <v>2030.67</v>
+        <f t="shared" ref="E37:G37" si="5">E34/2*E28/2*9.81</f>
+        <v>507.66750000000002</v>
       </c>
       <c r="F37" s="6">
-        <f>F34*F28*9.81</f>
-        <v>1412.64</v>
+        <f t="shared" si="5"/>
+        <v>353.16</v>
       </c>
       <c r="G37" s="6">
-        <f>G34*G28*9.81</f>
-        <v>2982.2400000000002</v>
+        <f t="shared" si="5"/>
+        <v>745.56000000000006</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B38" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D38" s="6">
-        <f>D12/1000*$C$5*D28/2*9.81</f>
-        <v>2383.83</v>
+        <f>D12/1000*$C$5*D28/2*9.81/2</f>
+        <v>1191.915</v>
       </c>
       <c r="E38" s="6">
-        <f>E12/1000*$C$5*E28/2*9.81</f>
-        <v>1462.0824</v>
+        <f t="shared" ref="E38:G38" si="6">E12/1000*$C$5*E28/2*9.81/2</f>
+        <v>731.0412</v>
       </c>
       <c r="F38" s="6">
-        <f>F12/1000*$C$5*F28/2*9.81</f>
-        <v>635.68799999999999</v>
+        <f t="shared" si="6"/>
+        <v>317.84399999999999</v>
       </c>
       <c r="G38" s="6">
-        <f>G12/1000*$C$5*G28/2*9.81</f>
-        <v>1342.0080000000003</v>
+        <f t="shared" si="6"/>
+        <v>671.00400000000013</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B39" s="5" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D39" s="6">
-        <f>2*D35*9.81</f>
-        <v>981</v>
+        <f>D35*9.81</f>
+        <v>490.5</v>
       </c>
       <c r="E39" s="6">
-        <f t="shared" ref="E39:G39" si="4">2*E35*9.81</f>
-        <v>981</v>
+        <f t="shared" ref="E39:G39" si="7">E35*9.81</f>
+        <v>490.5</v>
       </c>
       <c r="F39" s="6">
-        <f t="shared" si="4"/>
-        <v>981</v>
+        <f t="shared" si="7"/>
+        <v>490.5</v>
       </c>
       <c r="G39" s="6">
-        <f t="shared" si="4"/>
-        <v>981</v>
+        <f t="shared" si="7"/>
+        <v>490.5</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B40" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D40" s="6">
         <f>0.05*SUM(D36:D39)</f>
-        <v>741.67650000000003</v>
+        <v>227.59200000000001</v>
       </c>
       <c r="E40" s="6">
-        <f t="shared" ref="E40:G40" si="5">0.05*SUM(E36:E39)</f>
-        <v>674.48761999999999</v>
+        <f t="shared" ref="E40:G40" si="8">0.05*SUM(E36:E39)</f>
+        <v>199.27543500000002</v>
       </c>
       <c r="F40" s="6">
-        <f t="shared" si="5"/>
-        <v>592.46640000000002</v>
+        <f t="shared" si="8"/>
+        <v>168.43770000000001</v>
       </c>
       <c r="G40" s="6">
-        <f t="shared" si="5"/>
-        <v>730.76240000000007</v>
+        <f t="shared" si="8"/>
+        <v>211.84695000000002</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B41" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D41" s="6">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="E41" s="6">
-        <v>0</v>
+        <v>2001</v>
       </c>
       <c r="F41" s="6">
-        <v>0</v>
+        <v>2002</v>
       </c>
       <c r="G41" s="6">
-        <v>0</v>
+        <v>2003</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B42" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D42" s="6">
         <f>1.4*$C$4*9.81</f>
         <v>824.04000000000008</v>
       </c>
       <c r="E42" s="6">
-        <f>1.4*$C$4*9.81</f>
+        <f t="shared" ref="E42:G42" si="9">1.4*$C$4*9.81</f>
         <v>824.04000000000008</v>
       </c>
       <c r="F42" s="6">
-        <f>1.4*$C$4*9.81</f>
+        <f t="shared" si="9"/>
         <v>824.04000000000008</v>
       </c>
       <c r="G42" s="6">
-        <f>1.4*$C$4*9.81</f>
+        <f t="shared" si="9"/>
         <v>824.04000000000008</v>
       </c>
       <c r="H42" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B43" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D43" s="14">
-        <f>SUM(D34:D42)*0.001</f>
-        <v>16.458246500000001</v>
+        <f>SUM(D36:D42)*0.001</f>
+        <v>7.603472</v>
       </c>
       <c r="E43" s="14">
-        <f t="shared" ref="E43:G43" si="6">SUM(E34:E42)*0.001</f>
-        <v>15.047280020000001</v>
+        <f t="shared" ref="E43:G43" si="10">SUM(E36:E42)*0.001</f>
+        <v>7.0098241349999997</v>
       </c>
       <c r="F43" s="14">
-        <f t="shared" si="6"/>
-        <v>13.323834400000001</v>
+        <f t="shared" si="10"/>
+        <v>6.3632316999999992</v>
       </c>
       <c r="G43" s="14">
-        <f t="shared" si="6"/>
-        <v>16.228050400000001</v>
+        <f t="shared" si="10"/>
+        <v>7.2758259500000007</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B44" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D44" s="14">
         <f>(D38+D40+D42)*0.001</f>
-        <v>3.9495464999999998</v>
+        <v>2.243547</v>
       </c>
       <c r="E44" s="14">
-        <f t="shared" ref="E44:G44" si="7">(E38+E40+E42)*0.001</f>
-        <v>2.9606100200000003</v>
+        <f t="shared" ref="E44:G44" si="11">(E38+E40+E42)*0.001</f>
+        <v>1.7543566350000002</v>
       </c>
       <c r="F44" s="14">
-        <f t="shared" si="7"/>
-        <v>2.0521943999999999</v>
+        <f t="shared" si="11"/>
+        <v>1.3103217</v>
       </c>
       <c r="G44" s="14">
-        <f t="shared" si="7"/>
-        <v>2.8968104000000006</v>
+        <f t="shared" si="11"/>
+        <v>1.7068909500000002</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
@@ -3511,7 +3526,7 @@
     <row r="46" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B46" s="25"/>
       <c r="C46" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D46" s="20">
         <v>0.9</v>
@@ -3530,7 +3545,7 @@
     <row r="47" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B47" s="25"/>
       <c r="C47" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D47" s="20">
         <v>0.8</v>
@@ -3549,32 +3564,33 @@
     <row r="48" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="8"/>
       <c r="C48" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D48" s="15">
         <f>D44*D18/(D46*D47)</f>
-        <v>5.0791493055555552</v>
+        <v>2.8852199074074067</v>
       </c>
       <c r="E48" s="15">
         <f>E44*E18/(E46*E47)</f>
-        <v>6.3456147548010966</v>
-      </c>
-      <c r="F48" s="36">
+        <v>3.7601951195987651</v>
+      </c>
+      <c r="F48" s="30">
         <f>F44*F18/(F46*F47)</f>
-        <v>9.8967708333333295</v>
+        <v>6.3190668402777765</v>
       </c>
       <c r="G48" s="15">
         <f>G44*G18/(G46*G47)</f>
-        <v>6.9849787808641972</v>
+        <v>4.1157671440972221</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B32:H32"/>
     <mergeCell ref="C22:C24"/>
+    <mergeCell ref="I20:L20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>